<commit_message>
Commit with org change
</commit_message>
<xml_diff>
--- a/TestData/TestCaseExample.xlsx
+++ b/TestData/TestCaseExample.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="2"/>
+    <workbookView windowWidth="9240" windowHeight="4727" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -196,7 +196,7 @@
     <t>Contacts</t>
   </si>
   <si>
-    <t>Facebooks_</t>
+    <t>TataBooks_</t>
   </si>
   <si>
     <t>Chemicals</t>
@@ -926,6 +926,13 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>